<commit_message>
Assosiativity of equal and not equal in precedence.
</commit_message>
<xml_diff>
--- a/docs/Precedence_table.xlsx
+++ b/docs/Precedence_table.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="34">
   <si>
     <t xml:space="preserve">+</t>
   </si>
@@ -119,6 +119,9 @@
   </si>
   <si>
     <t xml:space="preserve">E → !E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">boolop</t>
   </si>
 </sst>
 </file>
@@ -128,7 +131,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -183,13 +186,21 @@
     <font>
       <b val="true"/>
       <sz val="15"/>
+      <color rgb="FF00CC33"/>
+      <name val="Arial Black"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="15"/>
       <color rgb="FFFF3333"/>
       <name val="Arial Black"/>
       <family val="2"/>
       <charset val="238"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -211,13 +222,19 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD9D9D9"/>
-        <bgColor rgb="FFC0C0C0"/>
+        <bgColor rgb="FFCCCCCC"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF99FF33"/>
         <bgColor rgb="FFCCFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCCCCC"/>
+        <bgColor rgb="FFD9D9D9"/>
       </patternFill>
     </fill>
   </fills>
@@ -262,7 +279,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -311,11 +328,23 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -333,7 +362,7 @@
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
       <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF00CC33"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
@@ -344,7 +373,7 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FFCCCCCC"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
@@ -396,17 +425,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AL18"/>
+  <dimension ref="A1:AL20"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L16" activeCellId="0" sqref="L16"/>
+      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.55"/>
   <cols>
-    <col collapsed="false" hidden="false" max="21" min="1" style="1" width="4.82186234817814"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="2" width="38.0040485829959"/>
-    <col collapsed="false" hidden="false" max="1025" min="23" style="1" width="4.82186234817814"/>
+    <col collapsed="false" hidden="false" max="21" min="1" style="1" width="4.78542510121457"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="2" width="38.0283400809717"/>
+    <col collapsed="false" hidden="false" max="1025" min="23" style="1" width="4.78542510121457"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -462,6 +491,24 @@
       <c r="R1" s="4" t="s">
         <v>16</v>
       </c>
+      <c r="U1" s="0"/>
+      <c r="V1" s="0"/>
+      <c r="W1" s="0"/>
+      <c r="X1" s="0"/>
+      <c r="Y1" s="0"/>
+      <c r="Z1" s="0"/>
+      <c r="AA1" s="0"/>
+      <c r="AB1" s="0"/>
+      <c r="AC1" s="0"/>
+      <c r="AD1" s="0"/>
+      <c r="AE1" s="0"/>
+      <c r="AF1" s="0"/>
+      <c r="AG1" s="0"/>
+      <c r="AH1" s="0"/>
+      <c r="AI1" s="0"/>
+      <c r="AJ1" s="0"/>
+      <c r="AK1" s="0"/>
+      <c r="AL1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
@@ -522,6 +569,22 @@
       <c r="V2" s="9" t="s">
         <v>17</v>
       </c>
+      <c r="W2" s="0"/>
+      <c r="X2" s="0"/>
+      <c r="Y2" s="0"/>
+      <c r="Z2" s="0"/>
+      <c r="AA2" s="0"/>
+      <c r="AB2" s="0"/>
+      <c r="AC2" s="0"/>
+      <c r="AD2" s="0"/>
+      <c r="AE2" s="0"/>
+      <c r="AF2" s="0"/>
+      <c r="AG2" s="0"/>
+      <c r="AH2" s="0"/>
+      <c r="AI2" s="0"/>
+      <c r="AJ2" s="0"/>
+      <c r="AK2" s="0"/>
+      <c r="AL2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
@@ -590,10 +653,12 @@
       <c r="AC3" s="10"/>
       <c r="AD3" s="10"/>
       <c r="AE3" s="10"/>
+      <c r="AF3" s="0"/>
       <c r="AG3" s="10"/>
       <c r="AH3" s="10"/>
       <c r="AI3" s="10"/>
       <c r="AJ3" s="8"/>
+      <c r="AK3" s="0"/>
       <c r="AL3" s="10"/>
     </row>
     <row r="4" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -663,10 +728,12 @@
       <c r="AC4" s="10"/>
       <c r="AD4" s="10"/>
       <c r="AE4" s="10"/>
+      <c r="AF4" s="0"/>
       <c r="AG4" s="10"/>
       <c r="AH4" s="10"/>
       <c r="AI4" s="10"/>
       <c r="AJ4" s="8"/>
+      <c r="AK4" s="0"/>
       <c r="AL4" s="10"/>
     </row>
     <row r="5" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -736,10 +803,12 @@
       <c r="AC5" s="10"/>
       <c r="AD5" s="10"/>
       <c r="AE5" s="10"/>
+      <c r="AF5" s="0"/>
       <c r="AG5" s="10"/>
       <c r="AH5" s="10"/>
       <c r="AI5" s="10"/>
       <c r="AJ5" s="8"/>
+      <c r="AK5" s="0"/>
       <c r="AL5" s="10"/>
     </row>
     <row r="6" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -801,10 +870,12 @@
       <c r="AC6" s="10"/>
       <c r="AD6" s="10"/>
       <c r="AE6" s="10"/>
+      <c r="AF6" s="0"/>
       <c r="AG6" s="10"/>
       <c r="AH6" s="10"/>
       <c r="AI6" s="10"/>
       <c r="AJ6" s="8"/>
+      <c r="AK6" s="0"/>
       <c r="AL6" s="10"/>
     </row>
     <row r="7" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -857,12 +928,21 @@
       <c r="V7" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="W7" s="0"/>
+      <c r="X7" s="0"/>
+      <c r="Y7" s="0"/>
+      <c r="Z7" s="0"/>
+      <c r="AA7" s="0"/>
+      <c r="AB7" s="0"/>
+      <c r="AC7" s="0"/>
       <c r="AD7" s="10"/>
       <c r="AE7" s="10"/>
+      <c r="AF7" s="0"/>
       <c r="AG7" s="10"/>
       <c r="AH7" s="10"/>
       <c r="AI7" s="10"/>
       <c r="AJ7" s="8"/>
+      <c r="AK7" s="0"/>
       <c r="AL7" s="10"/>
     </row>
     <row r="8" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -915,12 +995,21 @@
       <c r="V8" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="W8" s="0"/>
+      <c r="X8" s="0"/>
+      <c r="Y8" s="0"/>
+      <c r="Z8" s="0"/>
+      <c r="AA8" s="0"/>
+      <c r="AB8" s="0"/>
+      <c r="AC8" s="0"/>
       <c r="AD8" s="10"/>
       <c r="AE8" s="10"/>
+      <c r="AF8" s="0"/>
       <c r="AG8" s="10"/>
       <c r="AH8" s="10"/>
       <c r="AI8" s="10"/>
       <c r="AJ8" s="8"/>
+      <c r="AK8" s="0"/>
       <c r="AL8" s="10"/>
     </row>
     <row r="9" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -973,12 +1062,21 @@
       <c r="V9" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="W9" s="0"/>
+      <c r="X9" s="0"/>
+      <c r="Y9" s="0"/>
+      <c r="Z9" s="0"/>
+      <c r="AA9" s="0"/>
+      <c r="AB9" s="0"/>
+      <c r="AC9" s="0"/>
       <c r="AD9" s="10"/>
       <c r="AE9" s="10"/>
+      <c r="AF9" s="0"/>
       <c r="AG9" s="10"/>
       <c r="AH9" s="10"/>
       <c r="AI9" s="10"/>
       <c r="AJ9" s="8"/>
+      <c r="AK9" s="0"/>
       <c r="AL9" s="10"/>
     </row>
     <row r="10" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1009,8 +1107,12 @@
       <c r="I10" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11"/>
+      <c r="J10" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="K10" s="12" t="s">
+        <v>5</v>
+      </c>
       <c r="L10" s="7" t="s">
         <v>4</v>
       </c>
@@ -1035,12 +1137,21 @@
       <c r="V10" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="W10" s="0"/>
+      <c r="X10" s="0"/>
+      <c r="Y10" s="0"/>
+      <c r="Z10" s="0"/>
+      <c r="AA10" s="0"/>
+      <c r="AB10" s="0"/>
+      <c r="AC10" s="0"/>
       <c r="AD10" s="10"/>
       <c r="AE10" s="10"/>
+      <c r="AF10" s="0"/>
       <c r="AG10" s="10"/>
       <c r="AH10" s="10"/>
       <c r="AI10" s="10"/>
       <c r="AJ10" s="8"/>
+      <c r="AK10" s="0"/>
       <c r="AL10" s="10"/>
     </row>
     <row r="11" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1071,8 +1182,12 @@
       <c r="I11" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="J11" s="11"/>
-      <c r="K11" s="11"/>
+      <c r="J11" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="K11" s="12" t="s">
+        <v>5</v>
+      </c>
       <c r="L11" s="7" t="s">
         <v>4</v>
       </c>
@@ -1097,10 +1212,21 @@
       <c r="V11" s="2" t="s">
         <v>26</v>
       </c>
+      <c r="W11" s="0"/>
+      <c r="X11" s="0"/>
+      <c r="Y11" s="0"/>
+      <c r="Z11" s="0"/>
+      <c r="AA11" s="0"/>
+      <c r="AB11" s="0"/>
+      <c r="AC11" s="0"/>
+      <c r="AD11" s="0"/>
+      <c r="AE11" s="0"/>
+      <c r="AF11" s="0"/>
       <c r="AG11" s="10"/>
       <c r="AH11" s="10"/>
       <c r="AI11" s="10"/>
       <c r="AJ11" s="8"/>
+      <c r="AK11" s="0"/>
       <c r="AL11" s="10"/>
     </row>
     <row r="12" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1140,7 +1266,7 @@
       <c r="L12" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="M12" s="12" t="s">
+      <c r="M12" s="13" t="s">
         <v>27</v>
       </c>
       <c r="N12" s="6" t="s">
@@ -1159,10 +1285,21 @@
       <c r="V12" s="2" t="s">
         <v>28</v>
       </c>
+      <c r="W12" s="0"/>
+      <c r="X12" s="0"/>
+      <c r="Y12" s="0"/>
+      <c r="Z12" s="0"/>
+      <c r="AA12" s="0"/>
+      <c r="AB12" s="0"/>
+      <c r="AC12" s="0"/>
+      <c r="AD12" s="0"/>
+      <c r="AE12" s="0"/>
+      <c r="AF12" s="0"/>
       <c r="AG12" s="10"/>
       <c r="AH12" s="10"/>
       <c r="AI12" s="10"/>
       <c r="AJ12" s="8"/>
+      <c r="AK12" s="0"/>
       <c r="AL12" s="10"/>
     </row>
     <row r="13" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1219,9 +1356,22 @@
       <c r="V13" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="W13" s="0"/>
+      <c r="X13" s="0"/>
+      <c r="Y13" s="0"/>
+      <c r="Z13" s="0"/>
+      <c r="AA13" s="0"/>
+      <c r="AB13" s="0"/>
+      <c r="AC13" s="0"/>
+      <c r="AD13" s="0"/>
+      <c r="AE13" s="0"/>
+      <c r="AF13" s="0"/>
+      <c r="AG13" s="0"/>
       <c r="AH13" s="8"/>
       <c r="AI13" s="8"/>
       <c r="AJ13" s="8"/>
+      <c r="AK13" s="0"/>
+      <c r="AL13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
@@ -1290,10 +1440,12 @@
       <c r="AC14" s="10"/>
       <c r="AD14" s="10"/>
       <c r="AE14" s="10"/>
+      <c r="AF14" s="0"/>
       <c r="AG14" s="10"/>
       <c r="AH14" s="10"/>
       <c r="AI14" s="10"/>
       <c r="AJ14" s="10"/>
+      <c r="AK14" s="0"/>
       <c r="AL14" s="10"/>
     </row>
     <row r="15" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1577,8 +1729,15 @@
       <c r="AG18" s="10"/>
       <c r="AH18" s="10"/>
       <c r="AI18" s="10"/>
-      <c r="AJ18" s="13"/>
+      <c r="AJ18" s="14"/>
       <c r="AL18" s="10"/>
+    </row>
+    <row r="20" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="15"/>
+      <c r="B20" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="15"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
I don't what I did.
</commit_message>
<xml_diff>
--- a/docs/Precedence_table.xlsx
+++ b/docs/Precedence_table.xlsx
@@ -428,14 +428,14 @@
   <dimension ref="A1:AL20"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.55"/>
   <cols>
-    <col collapsed="false" hidden="false" max="21" min="1" style="1" width="4.78542510121457"/>
+    <col collapsed="false" hidden="false" max="21" min="1" style="1" width="4.66396761133603"/>
     <col collapsed="false" hidden="false" max="22" min="22" style="2" width="38.0283400809717"/>
-    <col collapsed="false" hidden="false" max="1025" min="23" style="1" width="4.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1025" min="23" style="1" width="4.66396761133603"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1732,6 +1732,11 @@
       <c r="AJ18" s="14"/>
       <c r="AL18" s="10"/>
     </row>
+    <row r="19" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0"/>
+      <c r="B19" s="0"/>
+      <c r="C19" s="0"/>
+    </row>
     <row r="20" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="15"/>
       <c r="B20" s="16" t="s">

</xml_diff>